<commit_message>
POSE extraction. Marker dictionaries added
</commit_message>
<xml_diff>
--- a/Simulations/Tests/Test.xlsx
+++ b/Simulations/Tests/Test.xlsx
@@ -9,15 +9,16 @@
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="mult_markers" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="fast" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="90deg" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Stereo" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Rotation_new" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="roll_and_pitch_new" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Lin_New" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Test_1_rotation" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Test_1a" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="mult_dict" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="mult_markers" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="fast" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="90deg" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Stereo" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Rotation_new" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="roll_and_pitch_new" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Lin_New" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Test_1_rotation" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Test_1a" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -85,22 +86,25 @@
     <t xml:space="preserve">0,0,0,0,0,0</t>
   </si>
   <si>
+    <t xml:space="preserve">DICT_5X5_50_s200_id0.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.25,0,0.1,0,0.52,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">models</t>
+  </si>
+  <si>
     <t xml:space="preserve">DICT_4X4_50_s100_id1.sdf</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.25,0,0.1,0,0.52,0</t>
-  </si>
-  <si>
     <t xml:space="preserve">DICT_4X4_50_s500_id2.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">0.3,0.3,0,0,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">models</t>
   </si>
   <si>
     <t xml:space="preserve">fast.txt</t>
@@ -252,7 +256,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -305,10 +309,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -331,7 +335,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,7 +343,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -379,20 +383,129 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -411,13 +524,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -498,21 +611,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -531,13 +636,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -560,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -605,23 +710,34 @@
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -643,10 +759,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -669,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,7 +793,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -712,25 +828,25 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -752,10 +868,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -778,7 +894,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +926,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -821,25 +937,25 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -861,10 +977,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -887,7 +1003,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,7 +1011,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,7 +1035,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -935,26 +1051,26 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -970,10 +1086,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -996,7 +1112,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,26 +1160,26 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1079,10 +1195,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -1153,20 +1269,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1188,10 +1304,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -1246,7 +1362,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -1262,20 +1378,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mvmnt File degree/radian option added. Pose extraction for mult markers added
</commit_message>
<xml_diff>
--- a/Simulations/Tests/Test.xlsx
+++ b/Simulations/Tests/Test.xlsx
@@ -9,16 +9,17 @@
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="mult_dict" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="mult_markers" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="fast" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="90deg" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Stereo" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Rotation_new" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="roll_and_pitch_new" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Lin_New" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Test_1_rotation" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Test_1a" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="many_markers" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="mult_dict" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="mult_markers" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="fast" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="90deg" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Stereo" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Rotation_new" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="roll_and_pitch_new" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Lin_New" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Test_1_rotation" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Test_1a" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="53">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -56,48 +57,90 @@
     <t xml:space="preserve">movement_file</t>
   </si>
   <si>
+    <t xml:space="preserve">many_markers.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gz_pose_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vid_pose_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cameras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KahnPhone_new.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,1,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">markers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0,0,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s500_id1.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7,0.2,0,0,0,0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s1000_id3.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,-2.3,0.8,-0.5,0.3,0.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id9.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.1,-0.2,0.1,-0.2,0.2,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id5.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,0,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_5X5_50_s100_id0.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,0.5,1,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_5X5_50_s200_id8.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.2,0.5,0,0,-0.53,2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_5X5_50_s100_id4.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.25,0,0.1,0,0.52,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">models</t>
+  </si>
+  <si>
     <t xml:space="preserve">mulp_markers.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">video_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gz_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vid_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cameras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KahnPhone_new.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1,1,0,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">markers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0,0,0,0,0</t>
-  </si>
-  <si>
     <t xml:space="preserve">DICT_5X5_50_s200_id0.sdf</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.25,0,0.1,0,0.52,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">models</t>
-  </si>
-  <si>
     <t xml:space="preserve">DICT_4X4_50_s100_id1.sdf</t>
   </si>
   <si>
@@ -120,9 +163,6 @@
   </si>
   <si>
     <t xml:space="preserve">DICT_4X4_50_s500_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s500_id1.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">Cam_Stereo_temp.sdf</t>
@@ -309,6 +349,115 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -335,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -383,20 +532,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -410,7 +559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -444,7 +593,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,7 +625,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -492,20 +641,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -524,9 +673,169 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -553,7 +862,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,20 +913,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -631,7 +940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -665,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,28 +1025,28 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +1060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -785,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,20 +1142,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +1169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -894,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,7 +1235,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -937,25 +1246,25 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -969,7 +1278,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1003,7 +1312,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,7 +1344,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -1051,20 +1360,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1078,7 +1387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1112,7 +1421,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1160,20 +1469,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1221,7 +1530,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,129 +1578,20 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>